<commit_message>
added a gif for family services over time and published again.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/vce-youth.xlsx
+++ b/ShinyApp/data/vce-youth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C909C-16C1-2F40-8CE3-040F5CE00AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9CA6D9-69C7-B944-9D7C-4875117211EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="15940" xr2:uid="{CDC3618B-1547-DD40-8FD4-89BB34720546}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t>Number</t>
   </si>
@@ -102,18 +102,6 @@
     <t xml:space="preserve">Public Benefits </t>
   </si>
   <si>
-    <t>14-18</t>
-  </si>
-  <si>
-    <t>19-21</t>
-  </si>
-  <si>
-    <t>22-29</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -124,6 +112,12 @@
   </si>
   <si>
     <t>Transitional housing</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>WRC</t>
   </si>
 </sst>
 </file>
@@ -133,7 +127,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -213,13 +207,13 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -230,6 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -546,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DB646B-5AE0-7549-96EE-01094861019E}">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +599,7 @@
         <v>19</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>0</v>
@@ -616,7 +611,7 @@
         <v>19</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AB1" s="12" t="s">
         <v>0</v>
@@ -693,19 +688,19 @@
         <v>2016</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W2" s="8">
-        <v>35</v>
-      </c>
-      <c r="X2" s="9">
-        <v>3.4584980237154152E-2</v>
+        <v>259</v>
+      </c>
+      <c r="X2" s="15">
+        <v>0</v>
       </c>
       <c r="Y2" s="7">
         <v>2015</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AB2" s="12">
         <v>38</v>
@@ -783,19 +778,20 @@
         <v>2016</v>
       </c>
       <c r="V3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="8">
+        <v>250</v>
+      </c>
+      <c r="X3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="7">
+        <f>Y2+1</f>
+        <v>2016</v>
+      </c>
+      <c r="AA3" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="W3" s="8">
-        <v>49</v>
-      </c>
-      <c r="X3" s="9">
-        <v>4.8418972332015808E-2</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>2015</v>
-      </c>
-      <c r="AA3" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="AB3" s="12">
         <v>32</v>
@@ -860,19 +856,20 @@
         <v>2016</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="W4" s="8">
-        <v>175</v>
-      </c>
-      <c r="X4" s="9">
-        <v>0.17292490118577075</v>
+        <v>275</v>
+      </c>
+      <c r="X4" s="15">
+        <v>0</v>
       </c>
       <c r="Y4" s="7">
-        <v>2015</v>
+        <f t="shared" ref="Y4:Y6" si="0">Y3+1</f>
+        <v>2017</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AB4" s="12">
         <v>35</v>
@@ -931,19 +928,20 @@
         <v>2017</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W5" s="8">
-        <v>26</v>
-      </c>
-      <c r="X5" s="9">
-        <v>2.5691699604743084E-2</v>
+        <v>319</v>
+      </c>
+      <c r="X5" s="15">
+        <v>0</v>
       </c>
       <c r="Y5" s="7">
-        <v>2016</v>
+        <f t="shared" si="0"/>
+        <v>2018</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AB5" s="13">
         <v>28</v>
@@ -952,7 +950,7 @@
         <v>2020</v>
       </c>
       <c r="AE5" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AF5" s="8">
         <v>13</v>
@@ -996,16 +994,17 @@
         <v>2017</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="W6" s="8">
-        <v>69</v>
-      </c>
-      <c r="X6" s="9">
-        <v>6.8181818181818177E-2</v>
+        <v>269</v>
+      </c>
+      <c r="X6" s="15">
+        <v>0</v>
       </c>
       <c r="Y6" s="7">
-        <v>2016</v>
+        <f t="shared" si="0"/>
+        <v>2019</v>
       </c>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
@@ -1041,18 +1040,10 @@
       <c r="T7" s="4">
         <v>2017</v>
       </c>
-      <c r="V7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="W7" s="8">
-        <v>155</v>
-      </c>
-      <c r="X7" s="9">
-        <v>0.15316205533596838</v>
-      </c>
-      <c r="Y7" s="7">
-        <v>2016</v>
-      </c>
+      <c r="V7" s="7"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
@@ -1071,18 +1062,10 @@
       <c r="T8" s="4">
         <v>2018</v>
       </c>
-      <c r="V8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W8" s="8">
-        <v>31</v>
-      </c>
-      <c r="X8" s="9">
-        <v>2.9865125240847785E-2</v>
-      </c>
-      <c r="Y8" s="7">
-        <v>2017</v>
-      </c>
+      <c r="V8" s="7"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -1110,18 +1093,10 @@
       <c r="T9" s="4">
         <v>2018</v>
       </c>
-      <c r="V9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W9" s="8">
-        <v>61</v>
-      </c>
-      <c r="X9" s="9">
-        <v>5.8766859344894028E-2</v>
-      </c>
-      <c r="Y9" s="7">
-        <v>2017</v>
-      </c>
+      <c r="V9" s="7"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
@@ -1149,20 +1124,12 @@
       <c r="T10" s="4">
         <v>2018</v>
       </c>
-      <c r="V10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="W10" s="8">
-        <v>183</v>
-      </c>
-      <c r="X10" s="9">
-        <v>0.17630057803468208</v>
-      </c>
-      <c r="Y10" s="7">
-        <v>2017</v>
-      </c>
+      <c r="V10" s="7"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="7"/>
       <c r="AE10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
@@ -1195,18 +1162,10 @@
       <c r="T11" s="4">
         <v>2019</v>
       </c>
-      <c r="V11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W11" s="8">
-        <v>41</v>
-      </c>
-      <c r="X11" s="9">
-        <v>4.2311661506707947E-2</v>
-      </c>
-      <c r="Y11" s="4">
-        <v>2018</v>
-      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
@@ -1225,18 +1184,10 @@
       <c r="T12" s="4">
         <v>2019</v>
       </c>
-      <c r="V12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W12" s="8">
-        <v>77</v>
-      </c>
-      <c r="X12" s="9">
-        <v>7.9463364293085662E-2</v>
-      </c>
-      <c r="Y12" s="4">
-        <v>2018</v>
-      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
@@ -1255,18 +1206,10 @@
       <c r="T13" s="4">
         <v>2019</v>
       </c>
-      <c r="V13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="W13" s="8">
-        <v>201</v>
-      </c>
-      <c r="X13" s="9">
-        <v>0.20743034055727555</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>2018</v>
-      </c>
+      <c r="V13" s="7"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
@@ -1285,18 +1228,10 @@
       <c r="T14" s="4">
         <v>2020</v>
       </c>
-      <c r="V14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W14" s="8">
-        <v>29</v>
-      </c>
-      <c r="X14" s="9">
-        <v>2.4390243902439025E-2</v>
-      </c>
-      <c r="Y14" s="4">
-        <v>2019</v>
-      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1315,18 +1250,10 @@
       <c r="T15" s="4">
         <v>2020</v>
       </c>
-      <c r="V15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W15" s="8">
-        <v>69</v>
-      </c>
-      <c r="X15" s="9">
-        <v>5.8031959629941128E-2</v>
-      </c>
-      <c r="Y15" s="4">
-        <v>2019</v>
-      </c>
+      <c r="V15" s="7"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -1345,18 +1272,10 @@
       <c r="T16" s="4">
         <v>2020</v>
       </c>
-      <c r="V16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="W16" s="8">
-        <v>171</v>
-      </c>
-      <c r="X16" s="9">
-        <v>0.1438183347350715</v>
-      </c>
-      <c r="Y16" s="4">
-        <v>2019</v>
-      </c>
+      <c r="V16" s="7"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="4"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
@@ -1364,8 +1283,8 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
       <c r="Y17" s="7"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -1374,7 +1293,20 @@
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CHange the ylabs as IB request. OVerview edits, add image of the wheel.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/vce-youth.xlsx
+++ b/ShinyApp/data/vce-youth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PhD\Internship\Loudoun\2021_DSPG_Loudoun\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0422B139-6573-A546-83C2-6A0BC25E2266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF9F89-6D29-43E3-AFD1-6F3A0D38057D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="15940" xr2:uid="{CDC3618B-1547-DD40-8FD4-89BB34720546}"/>
+    <workbookView xWindow="-23148" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{CDC3618B-1547-DD40-8FD4-89BB34720546}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Native Hawaiian</t>
   </si>
   <si>
-    <t>Indian</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>WRC</t>
+  </si>
+  <si>
+    <t>American Indian</t>
   </si>
 </sst>
 </file>
@@ -543,16 +543,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DB646B-5AE0-7549-96EE-01094861019E}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2:AF5"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -566,13 +566,13 @@
         <v>0</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -587,37 +587,37 @@
         <v>0</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
         <v>13</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>14</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>4</v>
@@ -632,16 +632,16 @@
         <v>0</v>
       </c>
       <c r="AK1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AM1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AM1" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -676,7 +676,7 @@
         <v>948</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R2" s="6">
         <v>5</v>
@@ -688,7 +688,7 @@
         <v>2016</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W2" s="8">
         <v>259</v>
@@ -700,7 +700,7 @@
         <v>2015</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB2" s="12">
         <v>38</v>
@@ -731,7 +731,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -766,7 +766,7 @@
         <v>1581</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R3" s="6">
         <v>111</v>
@@ -778,7 +778,7 @@
         <v>2016</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W3" s="8">
         <v>250</v>
@@ -791,7 +791,7 @@
         <v>2016</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB3" s="12">
         <v>32</v>
@@ -821,7 +821,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>372</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R4" s="6">
         <v>0</v>
@@ -856,7 +856,7 @@
         <v>2016</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W4" s="8">
         <v>275</v>
@@ -869,7 +869,7 @@
         <v>2017</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB4" s="12">
         <v>35</v>
@@ -893,9 +893,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -916,7 +916,7 @@
         <v>39</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R5" s="6">
         <v>53</v>
@@ -928,7 +928,7 @@
         <v>2017</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W5" s="8">
         <v>319</v>
@@ -941,7 +941,7 @@
         <v>2018</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB5" s="13">
         <v>28</v>
@@ -950,7 +950,7 @@
         <v>2020</v>
       </c>
       <c r="AE5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AF5" s="8">
         <v>13</v>
@@ -965,7 +965,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="G6" s="8">
         <v>27</v>
       </c>
@@ -976,13 +976,13 @@
         <v>2020</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="L6">
         <v>15</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R6" s="6">
         <v>200</v>
@@ -994,7 +994,7 @@
         <v>2017</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="8">
         <v>269</v>
@@ -1018,18 +1018,18 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L7">
         <v>222</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R7" s="6">
         <v>0</v>
@@ -1045,13 +1045,13 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="7"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="Q8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R8" s="6">
         <v>21</v>
@@ -1067,7 +1067,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="7"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1082,7 +1082,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="Q9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R9" s="6">
         <v>296</v>
@@ -1098,7 +1098,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="6"/>
@@ -1113,7 +1113,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="2"/>
       <c r="Q10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R10" s="6">
         <v>1</v>
@@ -1129,12 +1129,12 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="7"/>
       <c r="AE10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -1147,11 +1147,11 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" s="1"/>
       <c r="Q11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R11" s="6">
         <v>68</v>
@@ -1167,13 +1167,13 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="7"/>
       <c r="Q12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R12" s="6">
         <v>758</v>
@@ -1189,13 +1189,13 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="7"/>
       <c r="Q13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R13" s="6">
         <v>4</v>
@@ -1211,13 +1211,13 @@
       <c r="X13" s="15"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="7"/>
       <c r="Q14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R14" s="6">
         <v>175</v>
@@ -1233,13 +1233,13 @@
       <c r="X14" s="15"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="Q15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R15" s="6">
         <v>832</v>
@@ -1255,13 +1255,13 @@
       <c r="X15" s="15"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="Q16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R16" s="6">
         <v>5</v>
@@ -1277,7 +1277,7 @@
       <c r="X16" s="15"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1287,7 +1287,7 @@
       <c r="X17" s="16"/>
       <c r="Y17" s="7"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="4"/>
       <c r="T18" s="7"/>
@@ -1296,15 +1296,15 @@
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
     </row>

</xml_diff>